<commit_message>
Nueva ejecución screenshots investing y yahoo
</commit_message>
<xml_diff>
--- a/Screenshots/_DCWebUrlFromNombreEmpresa.xlsx
+++ b/Screenshots/_DCWebUrlFromNombreEmpresa.xlsx
@@ -13598,11 +13598,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="___urls_yahoo_desde_google" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="new 2" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="new 2" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="___urls_yahoo_desde_google" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -45189,7 +45189,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="35" style="5" customWidth="1"/>
     <col min="2" max="2" width="70.28515625" style="5" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" style="5"/>
     <col min="4" max="4" width="70.28515625" style="5" customWidth="1"/>

</xml_diff>

<commit_message>
Añadidos nombres de empresa del Aristopack del barón del dividendo
</commit_message>
<xml_diff>
--- a/Screenshots/_DCWebUrlFromNombreEmpresa.xlsx
+++ b/Screenshots/_DCWebUrlFromNombreEmpresa.xlsx
@@ -674,7 +674,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9363" uniqueCount="4277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9408" uniqueCount="4321">
   <si>
     <t>-</t>
   </si>
@@ -13505,6 +13505,138 @@
   </si>
   <si>
     <t>https://es.investing.com/equities/shire-plc</t>
+  </si>
+  <si>
+    <t>ABB</t>
+  </si>
+  <si>
+    <t>Amplifon</t>
+  </si>
+  <si>
+    <t>Assa Abloy</t>
+  </si>
+  <si>
+    <t>BMO Global Smaller Companies</t>
+  </si>
+  <si>
+    <t>BlackRock Smaller Companies Trust</t>
+  </si>
+  <si>
+    <t>Chesapeake Financial Shares</t>
+  </si>
+  <si>
+    <t>Clarkson</t>
+  </si>
+  <si>
+    <t>Computacenter</t>
+  </si>
+  <si>
+    <t>DCC</t>
+  </si>
+  <si>
+    <t>Dajean Holdings</t>
+  </si>
+  <si>
+    <t>Diasorin</t>
+  </si>
+  <si>
+    <t>D’leteren</t>
+  </si>
+  <si>
+    <t>Emera Inc.</t>
+  </si>
+  <si>
+    <t>Experian</t>
+  </si>
+  <si>
+    <t>F&amp;C Investment Trust</t>
+  </si>
+  <si>
+    <t>Fidelity Special Values</t>
+  </si>
+  <si>
+    <t>Golden Ocean</t>
+  </si>
+  <si>
+    <t>HICL Infrastructure</t>
+  </si>
+  <si>
+    <t>Hiscox</t>
+  </si>
+  <si>
+    <t>Huhtamaki</t>
+  </si>
+  <si>
+    <t>IWG</t>
+  </si>
+  <si>
+    <t>Ibersol</t>
+  </si>
+  <si>
+    <t>Intermediate Capital Group</t>
+  </si>
+  <si>
+    <t>International Public Partnership</t>
+  </si>
+  <si>
+    <t>Investor</t>
+  </si>
+  <si>
+    <t>Kemira</t>
+  </si>
+  <si>
+    <t>Kinnevik</t>
+  </si>
+  <si>
+    <t>Lonza</t>
+  </si>
+  <si>
+    <t>Metro Inc.</t>
+  </si>
+  <si>
+    <t>Paragon Banking Group</t>
+  </si>
+  <si>
+    <t>Perpetual Income &amp; Growth IT</t>
+  </si>
+  <si>
+    <t>REN Red Energeticas Nacionais</t>
+  </si>
+  <si>
+    <t>Schroder Oriental Income Fund</t>
+  </si>
+  <si>
+    <t>Scottish Investment Trust</t>
+  </si>
+  <si>
+    <t>Scottish Mortgage Investment</t>
+  </si>
+  <si>
+    <t>Securitas</t>
+  </si>
+  <si>
+    <t>Svenska Enskilda Banken</t>
+  </si>
+  <si>
+    <t>Swedish Match</t>
+  </si>
+  <si>
+    <t>Swiss Re</t>
+  </si>
+  <si>
+    <t>UCB</t>
+  </si>
+  <si>
+    <t>UDG Healthcare</t>
+  </si>
+  <si>
+    <t>Witan Investment Trust</t>
+  </si>
+  <si>
+    <t>Wood Group</t>
+  </si>
+  <si>
+    <t>Zurich Insurances</t>
   </si>
 </sst>
 </file>
@@ -13607,11 +13739,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="___urls_yahoo_desde_google" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="new 2" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="new 2" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="___urls_yahoo_desde_google" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -45192,9 +45324,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D1086"/>
+  <dimension ref="B1:G1086"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:G47"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -45202,11 +45336,13 @@
     <col min="2" max="2" width="70.28515625" style="5" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" style="5"/>
     <col min="4" max="4" width="70.28515625" style="5" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="5"/>
+    <col min="5" max="6" width="11.42578125" style="5"/>
+    <col min="7" max="7" width="34.42578125" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:4" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:7" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:7" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="6" t="s">
         <v>4270</v>
       </c>
@@ -45214,367 +45350,502 @@
         <v>4271</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>4109</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>2281</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G3" s="5" t="s">
+        <v>4277</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>4091</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>2282</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G4" s="5" t="s">
+        <v>4278</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>3395</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>2283</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G5" s="5" t="s">
+        <v>4279</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>3466</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>2284</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G6" s="5" t="s">
+        <v>4280</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>3398</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>2285</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G7" s="5" t="s">
+        <v>4281</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
         <v>3399</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>3205</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G8" s="5" t="s">
+        <v>4282</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>3447</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>2338</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G9" s="5" t="s">
+        <v>4283</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
         <v>3401</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>2286</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G10" s="5" t="s">
+        <v>4284</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
         <v>3402</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>3202</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G11" s="5" t="s">
+        <v>4285</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
         <v>3439</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>2287</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G12" s="5" t="s">
+        <v>4286</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
         <v>3403</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>2288</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G13" s="5" t="s">
+        <v>4287</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
         <v>3460</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>2289</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G14" s="5" t="s">
+        <v>4288</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="s">
         <v>3445</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>3203</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G15" s="5" t="s">
+        <v>4289</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16" s="4" t="s">
         <v>3404</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>3204</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G16" s="5" t="s">
+        <v>4290</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="s">
         <v>3400</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>2290</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G17" s="5" t="s">
+        <v>4291</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="s">
         <v>3627</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>2291</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G18" s="5" t="s">
+        <v>4292</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" s="4" t="s">
         <v>3409</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>2292</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G19" s="5" t="s">
+        <v>4293</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="s">
         <v>3405</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>2293</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G20" s="5" t="s">
+        <v>4294</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" s="4" t="s">
         <v>3463</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>2294</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G21" s="5" t="s">
+        <v>4295</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B22" s="4" t="s">
         <v>3407</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>2295</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G22" s="5" t="s">
+        <v>4296</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23" s="4" t="s">
         <v>3411</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>2296</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G23" s="5" t="s">
+        <v>4297</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B24" s="4" t="s">
         <v>3410</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>2297</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G24" s="5" t="s">
+        <v>4298</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B25" s="4" t="s">
         <v>3408</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>2298</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G25" s="5" t="s">
+        <v>4299</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B26" s="4" t="s">
         <v>3420</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>2299</v>
       </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G26" s="5" t="s">
+        <v>4300</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B27" s="4" t="s">
         <v>3442</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>2300</v>
       </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G27" s="5" t="s">
+        <v>4301</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B28" s="4" t="s">
         <v>3452</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>3315</v>
       </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G28" s="5" t="s">
+        <v>4302</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B29" s="4" t="s">
         <v>3471</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>2301</v>
       </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G29" s="5" t="s">
+        <v>4303</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B30" s="4" t="s">
         <v>3413</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>2302</v>
       </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G30" s="5" t="s">
+        <v>4304</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B31" s="4" t="s">
         <v>3444</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>2303</v>
       </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G31" s="5" t="s">
+        <v>4305</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B32" s="4" t="s">
         <v>3414</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>3316</v>
       </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G32" s="5" t="s">
+        <v>4306</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B33" s="4" t="s">
         <v>2222</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>2304</v>
       </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G33" s="5" t="s">
+        <v>4307</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B34" s="4" t="s">
         <v>3416</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>2305</v>
       </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G34" s="5" t="s">
+        <v>4308</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B35" s="4" t="s">
         <v>3434</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>2306</v>
       </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G35" s="5" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B36" s="4" t="s">
         <v>3417</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>2307</v>
       </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G36" s="5" t="s">
+        <v>4309</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B37" s="4" t="s">
         <v>3415</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>2309</v>
       </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G37" s="5" t="s">
+        <v>4310</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B38" s="4" t="s">
         <v>3419</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>2310</v>
       </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G38" s="5" t="s">
+        <v>4311</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B39" s="4" t="s">
         <v>3421</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>2311</v>
       </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G39" s="5" t="s">
+        <v>4312</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B40" s="4" t="s">
         <v>3458</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>2312</v>
       </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G40" s="5" t="s">
+        <v>4313</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B41" s="4" t="s">
         <v>3422</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>2313</v>
       </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G41" s="5" t="s">
+        <v>4314</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B42" s="4" t="s">
         <v>3469</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>2314</v>
       </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G42" s="5" t="s">
+        <v>4315</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B43" s="4" t="s">
         <v>3423</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>2315</v>
       </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G43" s="5" t="s">
+        <v>4316</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B44" s="4" t="s">
         <v>3448</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>2316</v>
       </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G44" s="5" t="s">
+        <v>4317</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B45" s="4" t="s">
         <v>3461</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>2318</v>
       </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G45" s="5" t="s">
+        <v>4318</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B46" s="4" t="s">
         <v>3453</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>2317</v>
       </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G46" s="5" t="s">
+        <v>4319</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B47" s="4" t="s">
         <v>3424</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>3293</v>
       </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G47" s="5" t="s">
+        <v>4320</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B48" s="4" t="s">
         <v>3425</v>
       </c>

</xml_diff>

<commit_message>
Nueva ejecucion proceso. Incluidas empresas Aristopack (Barón del dividendo)
</commit_message>
<xml_diff>
--- a/Screenshots/_DCWebUrlFromNombreEmpresa.xlsx
+++ b/Screenshots/_DCWebUrlFromNombreEmpresa.xlsx
@@ -674,7 +674,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9408" uniqueCount="4321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9404" uniqueCount="4317">
   <si>
     <t>-</t>
   </si>
@@ -13507,136 +13507,124 @@
     <t>https://es.investing.com/equities/shire-plc</t>
   </si>
   <si>
-    <t>ABB</t>
-  </si>
-  <si>
-    <t>Amplifon</t>
-  </si>
-  <si>
-    <t>Assa Abloy</t>
-  </si>
-  <si>
-    <t>BMO Global Smaller Companies</t>
-  </si>
-  <si>
-    <t>BlackRock Smaller Companies Trust</t>
-  </si>
-  <si>
-    <t>Chesapeake Financial Shares</t>
-  </si>
-  <si>
-    <t>Clarkson</t>
-  </si>
-  <si>
-    <t>Computacenter</t>
-  </si>
-  <si>
-    <t>DCC</t>
-  </si>
-  <si>
-    <t>Dajean Holdings</t>
-  </si>
-  <si>
-    <t>Diasorin</t>
-  </si>
-  <si>
-    <t>D’leteren</t>
-  </si>
-  <si>
-    <t>Emera Inc.</t>
-  </si>
-  <si>
-    <t>Experian</t>
-  </si>
-  <si>
-    <t>F&amp;C Investment Trust</t>
-  </si>
-  <si>
-    <t>Fidelity Special Values</t>
-  </si>
-  <si>
-    <t>Golden Ocean</t>
-  </si>
-  <si>
-    <t>HICL Infrastructure</t>
-  </si>
-  <si>
-    <t>Hiscox</t>
-  </si>
-  <si>
-    <t>Huhtamaki</t>
-  </si>
-  <si>
-    <t>IWG</t>
-  </si>
-  <si>
-    <t>Ibersol</t>
-  </si>
-  <si>
-    <t>Intermediate Capital Group</t>
-  </si>
-  <si>
-    <t>International Public Partnership</t>
-  </si>
-  <si>
-    <t>Investor</t>
-  </si>
-  <si>
-    <t>Kemira</t>
-  </si>
-  <si>
-    <t>Kinnevik</t>
-  </si>
-  <si>
-    <t>Lonza</t>
-  </si>
-  <si>
-    <t>Metro Inc.</t>
-  </si>
-  <si>
-    <t>Paragon Banking Group</t>
-  </si>
-  <si>
-    <t>Perpetual Income &amp; Growth IT</t>
-  </si>
-  <si>
-    <t>REN Red Energeticas Nacionais</t>
-  </si>
-  <si>
-    <t>Schroder Oriental Income Fund</t>
-  </si>
-  <si>
-    <t>Scottish Investment Trust</t>
-  </si>
-  <si>
-    <t>Scottish Mortgage Investment</t>
-  </si>
-  <si>
-    <t>Securitas</t>
-  </si>
-  <si>
-    <t>Svenska Enskilda Banken</t>
-  </si>
-  <si>
-    <t>Swedish Match</t>
-  </si>
-  <si>
-    <t>Swiss Re</t>
-  </si>
-  <si>
-    <t>UCB</t>
-  </si>
-  <si>
-    <t>UDG Healthcare</t>
-  </si>
-  <si>
-    <t>Witan Investment Trust</t>
-  </si>
-  <si>
-    <t>Wood Group</t>
-  </si>
-  <si>
-    <t>Zurich Insurances</t>
+    <t>https://es.investing.com/equities/abb-ltd</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/assa-abloy</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/f-c-global-smaller-companies-plc</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/blckrck-sm-co</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/chesapeake-finl-shs</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/clarkson-plc</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/computacenter</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/dcc-plc-exch</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/emera-incorporated</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/experian-ord-usd0</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/foreign-and-colonial-inv-trust</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/fidelity-special-values</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/knightsbridge-tankers-ltd</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/hicl-infrastructure</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/hiscox</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/huhtamaki</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/regus-group</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/intermediate-capital-group</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/intl-public-partnership</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/investors-bancorp</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/kemira-oy</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/kinnevik-investment-a</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/kinnevik-investment-b</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/lonza-grp</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/metro-inc</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/the-paragon-group-of-companies-plc</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/perpetual-inc---growth</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/skf</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/schroder-oriental-income-fund-ltd</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/scottish-investment-trust</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/scottish-mortgage-inv-trust</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/securitas-b</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/swedish-match</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/swiss-re</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/ucb</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/united-drug-plc</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/witan-investment-company</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/john-wood-group</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/zurich-fin</t>
+  </si>
+  <si>
+    <t>Aristopack (Barón del Dividendo):</t>
   </si>
 </sst>
 </file>
@@ -13739,11 +13727,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="new 2" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="___urls_yahoo_desde_google" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="___urls_yahoo_desde_google" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="new 2" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -45324,11 +45312,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G1086"/>
+  <dimension ref="B1:D1128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G47"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -45336,13 +45322,11 @@
     <col min="2" max="2" width="70.28515625" style="5" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" style="5"/>
     <col min="4" max="4" width="70.28515625" style="5" customWidth="1"/>
-    <col min="5" max="6" width="11.42578125" style="5"/>
-    <col min="7" max="7" width="34.42578125" style="5" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="5"/>
+    <col min="5" max="16384" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:7" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:4" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:4" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="6" t="s">
         <v>4270</v>
       </c>
@@ -45350,502 +45334,367 @@
         <v>4271</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>4109</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>2281</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>4277</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>4091</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>2282</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>4278</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>3395</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>2283</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>4279</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>3466</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>2284</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>4280</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>3398</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>2285</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>4281</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
         <v>3399</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>3205</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>4282</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>3447</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>2338</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>4283</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
         <v>3401</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>2286</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>4284</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
         <v>3402</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>3202</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>4285</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
         <v>3439</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>2287</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>4286</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
         <v>3403</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>2288</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>4287</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
         <v>3460</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>2289</v>
       </c>
-      <c r="G14" s="5" t="s">
-        <v>4288</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="s">
         <v>3445</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>3203</v>
       </c>
-      <c r="G15" s="5" t="s">
-        <v>4289</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B16" s="4" t="s">
         <v>3404</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>3204</v>
       </c>
-      <c r="G16" s="5" t="s">
-        <v>4290</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="s">
         <v>3400</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>2290</v>
       </c>
-      <c r="G17" s="5" t="s">
-        <v>4291</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="s">
         <v>3627</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>2291</v>
       </c>
-      <c r="G18" s="5" t="s">
-        <v>4292</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="4" t="s">
         <v>3409</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>2292</v>
       </c>
-      <c r="G19" s="5" t="s">
-        <v>4293</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="s">
         <v>3405</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>2293</v>
       </c>
-      <c r="G20" s="5" t="s">
-        <v>4294</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="4" t="s">
         <v>3463</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>2294</v>
       </c>
-      <c r="G21" s="5" t="s">
-        <v>4295</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="4" t="s">
         <v>3407</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>2295</v>
       </c>
-      <c r="G22" s="5" t="s">
-        <v>4296</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="4" t="s">
         <v>3411</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>2296</v>
       </c>
-      <c r="G23" s="5" t="s">
-        <v>4297</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="4" t="s">
         <v>3410</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>2297</v>
       </c>
-      <c r="G24" s="5" t="s">
-        <v>4298</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="4" t="s">
         <v>3408</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>2298</v>
       </c>
-      <c r="G25" s="5" t="s">
-        <v>4299</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="4" t="s">
         <v>3420</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>2299</v>
       </c>
-      <c r="G26" s="5" t="s">
-        <v>4300</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" s="4" t="s">
         <v>3442</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>2300</v>
       </c>
-      <c r="G27" s="5" t="s">
-        <v>4301</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="4" t="s">
         <v>3452</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>3315</v>
       </c>
-      <c r="G28" s="5" t="s">
-        <v>4302</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" s="4" t="s">
         <v>3471</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>2301</v>
       </c>
-      <c r="G29" s="5" t="s">
-        <v>4303</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" s="4" t="s">
         <v>3413</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>2302</v>
       </c>
-      <c r="G30" s="5" t="s">
-        <v>4304</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B31" s="4" t="s">
         <v>3444</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>2303</v>
       </c>
-      <c r="G31" s="5" t="s">
-        <v>4305</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32" s="4" t="s">
         <v>3414</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>3316</v>
       </c>
-      <c r="G32" s="5" t="s">
-        <v>4306</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="4" t="s">
         <v>2222</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>2304</v>
       </c>
-      <c r="G33" s="5" t="s">
-        <v>4307</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="4" t="s">
         <v>3416</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>2305</v>
       </c>
-      <c r="G34" s="5" t="s">
-        <v>4308</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="4" t="s">
         <v>3434</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>2306</v>
       </c>
-      <c r="G35" s="5" t="s">
-        <v>1229</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="4" t="s">
         <v>3417</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>2307</v>
       </c>
-      <c r="G36" s="5" t="s">
-        <v>4309</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="4" t="s">
         <v>3415</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>2309</v>
       </c>
-      <c r="G37" s="5" t="s">
-        <v>4310</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="4" t="s">
         <v>3419</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>2310</v>
       </c>
-      <c r="G38" s="5" t="s">
-        <v>4311</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="4" t="s">
         <v>3421</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>2311</v>
       </c>
-      <c r="G39" s="5" t="s">
-        <v>4312</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" s="4" t="s">
         <v>3458</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>2312</v>
       </c>
-      <c r="G40" s="5" t="s">
-        <v>4313</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B41" s="4" t="s">
         <v>3422</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>2313</v>
       </c>
-      <c r="G41" s="5" t="s">
-        <v>4314</v>
-      </c>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" s="4" t="s">
         <v>3469</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>2314</v>
       </c>
-      <c r="G42" s="5" t="s">
-        <v>4315</v>
-      </c>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43" s="4" t="s">
         <v>3423</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>2315</v>
       </c>
-      <c r="G43" s="5" t="s">
-        <v>4316</v>
-      </c>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B44" s="4" t="s">
         <v>3448</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>2316</v>
       </c>
-      <c r="G44" s="5" t="s">
-        <v>4317</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" s="4" t="s">
         <v>3461</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>2318</v>
       </c>
-      <c r="G45" s="5" t="s">
-        <v>4318</v>
-      </c>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B46" s="4" t="s">
         <v>3453</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>2317</v>
       </c>
-      <c r="G46" s="5" t="s">
-        <v>4319</v>
-      </c>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B47" s="4" t="s">
         <v>3424</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>3293</v>
       </c>
-      <c r="G47" s="5" t="s">
-        <v>4320</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B48" s="4" t="s">
         <v>3425</v>
       </c>
@@ -53900,6 +53749,211 @@
     <row r="1086" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D1086" s="4" t="s">
         <v>3201</v>
+      </c>
+    </row>
+    <row r="1088" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1088" s="5" t="s">
+        <v>4316</v>
+      </c>
+    </row>
+    <row r="1089" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1089" s="4" t="s">
+        <v>4277</v>
+      </c>
+    </row>
+    <row r="1090" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1090" s="4" t="s">
+        <v>4278</v>
+      </c>
+    </row>
+    <row r="1091" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1091" s="4" t="s">
+        <v>4279</v>
+      </c>
+    </row>
+    <row r="1092" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1092" s="4" t="s">
+        <v>4280</v>
+      </c>
+    </row>
+    <row r="1093" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1093" s="4" t="s">
+        <v>4281</v>
+      </c>
+    </row>
+    <row r="1094" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1094" s="4" t="s">
+        <v>4282</v>
+      </c>
+    </row>
+    <row r="1095" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1095" s="4" t="s">
+        <v>4283</v>
+      </c>
+    </row>
+    <row r="1096" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1096" s="4" t="s">
+        <v>4284</v>
+      </c>
+    </row>
+    <row r="1097" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1097" s="4" t="s">
+        <v>4285</v>
+      </c>
+    </row>
+    <row r="1098" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1098" s="4" t="s">
+        <v>4286</v>
+      </c>
+    </row>
+    <row r="1099" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1099" s="4" t="s">
+        <v>4287</v>
+      </c>
+    </row>
+    <row r="1100" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1100" s="4" t="s">
+        <v>4288</v>
+      </c>
+    </row>
+    <row r="1101" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1101" s="4" t="s">
+        <v>4289</v>
+      </c>
+    </row>
+    <row r="1102" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1102" s="4" t="s">
+        <v>4290</v>
+      </c>
+    </row>
+    <row r="1103" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1103" s="4" t="s">
+        <v>4291</v>
+      </c>
+    </row>
+    <row r="1104" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1104" s="4" t="s">
+        <v>4292</v>
+      </c>
+    </row>
+    <row r="1105" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1105" s="4" t="s">
+        <v>4293</v>
+      </c>
+    </row>
+    <row r="1106" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1106" s="4" t="s">
+        <v>4294</v>
+      </c>
+    </row>
+    <row r="1107" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1107" s="4" t="s">
+        <v>4295</v>
+      </c>
+    </row>
+    <row r="1108" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1108" s="4" t="s">
+        <v>4296</v>
+      </c>
+    </row>
+    <row r="1109" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1109" s="4" t="s">
+        <v>4297</v>
+      </c>
+    </row>
+    <row r="1110" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1110" s="4" t="s">
+        <v>4298</v>
+      </c>
+    </row>
+    <row r="1111" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1111" s="4" t="s">
+        <v>4299</v>
+      </c>
+    </row>
+    <row r="1112" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1112" s="4" t="s">
+        <v>4300</v>
+      </c>
+    </row>
+    <row r="1113" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1113" s="4" t="s">
+        <v>4301</v>
+      </c>
+    </row>
+    <row r="1114" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1114" s="4" t="s">
+        <v>4302</v>
+      </c>
+    </row>
+    <row r="1115" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1115" s="4" t="s">
+        <v>4303</v>
+      </c>
+    </row>
+    <row r="1116" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1116" s="4" t="s">
+        <v>4304</v>
+      </c>
+    </row>
+    <row r="1117" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1117" s="4" t="s">
+        <v>4305</v>
+      </c>
+    </row>
+    <row r="1118" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1118" s="4" t="s">
+        <v>4306</v>
+      </c>
+    </row>
+    <row r="1119" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1119" s="4" t="s">
+        <v>4307</v>
+      </c>
+    </row>
+    <row r="1120" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1120" s="4" t="s">
+        <v>4308</v>
+      </c>
+    </row>
+    <row r="1121" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1121" s="4" t="s">
+        <v>3277</v>
+      </c>
+    </row>
+    <row r="1122" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1122" s="4" t="s">
+        <v>4309</v>
+      </c>
+    </row>
+    <row r="1123" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1123" s="4" t="s">
+        <v>4310</v>
+      </c>
+    </row>
+    <row r="1124" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1124" s="4" t="s">
+        <v>4311</v>
+      </c>
+    </row>
+    <row r="1125" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1125" s="4" t="s">
+        <v>4312</v>
+      </c>
+    </row>
+    <row r="1126" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1126" s="4" t="s">
+        <v>4313</v>
+      </c>
+    </row>
+    <row r="1127" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1127" s="4" t="s">
+        <v>4314</v>
+      </c>
+    </row>
+    <row r="1128" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D1128" s="4" t="s">
+        <v>4315</v>
       </c>
     </row>
   </sheetData>
@@ -53907,8 +53961,48 @@
     <hyperlink ref="D429" r:id="rId1"/>
     <hyperlink ref="D473" r:id="rId2"/>
     <hyperlink ref="D891" r:id="rId3"/>
+    <hyperlink ref="D1089" r:id="rId4"/>
+    <hyperlink ref="D1090" r:id="rId5"/>
+    <hyperlink ref="D1091" r:id="rId6"/>
+    <hyperlink ref="D1092" r:id="rId7"/>
+    <hyperlink ref="D1093" r:id="rId8"/>
+    <hyperlink ref="D1094" r:id="rId9"/>
+    <hyperlink ref="D1095" r:id="rId10"/>
+    <hyperlink ref="D1096" r:id="rId11"/>
+    <hyperlink ref="D1097" r:id="rId12"/>
+    <hyperlink ref="D1098" r:id="rId13"/>
+    <hyperlink ref="D1099" r:id="rId14"/>
+    <hyperlink ref="D1100" r:id="rId15"/>
+    <hyperlink ref="D1101" r:id="rId16"/>
+    <hyperlink ref="D1102" r:id="rId17"/>
+    <hyperlink ref="D1103" r:id="rId18"/>
+    <hyperlink ref="D1104" r:id="rId19"/>
+    <hyperlink ref="D1105" r:id="rId20"/>
+    <hyperlink ref="D1106" r:id="rId21"/>
+    <hyperlink ref="D1107" r:id="rId22"/>
+    <hyperlink ref="D1108" r:id="rId23"/>
+    <hyperlink ref="D1109" r:id="rId24"/>
+    <hyperlink ref="D1110" r:id="rId25"/>
+    <hyperlink ref="D1111" r:id="rId26"/>
+    <hyperlink ref="D1112" r:id="rId27"/>
+    <hyperlink ref="D1113" r:id="rId28"/>
+    <hyperlink ref="D1114" r:id="rId29"/>
+    <hyperlink ref="D1115" r:id="rId30"/>
+    <hyperlink ref="D1116" r:id="rId31"/>
+    <hyperlink ref="D1117" r:id="rId32"/>
+    <hyperlink ref="D1118" r:id="rId33"/>
+    <hyperlink ref="D1119" r:id="rId34"/>
+    <hyperlink ref="D1120" r:id="rId35"/>
+    <hyperlink ref="D1121" r:id="rId36"/>
+    <hyperlink ref="D1122" r:id="rId37"/>
+    <hyperlink ref="D1123" r:id="rId38"/>
+    <hyperlink ref="D1124" r:id="rId39"/>
+    <hyperlink ref="D1125" r:id="rId40"/>
+    <hyperlink ref="D1126" r:id="rId41"/>
+    <hyperlink ref="D1127" r:id="rId42"/>
+    <hyperlink ref="D1128" r:id="rId43"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId44"/>
 </worksheet>
 </file>
</xml_diff>